<commit_message>
BOM fix for RST switch
</commit_message>
<xml_diff>
--- a/hardware/Light_Rail_BOM.xlsx
+++ b/hardware/Light_Rail_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Light-Rail\hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\project\Light-Rail\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ED71E6-EA0E-4935-9EE1-323DAD1A4F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFFAC5D-5166-412E-9C3B-D388227EEF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21570" yWindow="-2110" windowWidth="21670" windowHeight="18470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,12 +304,6 @@
     <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
   </si>
   <si>
-    <t>PTS810SJS250SMTR LFS</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 16V</t>
-  </si>
-  <si>
     <t>C&amp;K</t>
   </si>
   <si>
@@ -452,6 +446,12 @@
   </si>
   <si>
     <t>T-P2W598827A BOM  (Light Rail Bill of Materials)</t>
+  </si>
+  <si>
+    <t>SKRKAGE020</t>
+  </si>
+  <si>
+    <t>SMD Tab</t>
   </si>
   <si>
     <t>SW13</t>
@@ -1004,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I37"/>
+  <dimension ref="A2:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1028,7 +1028,7 @@
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="D2" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
@@ -1083,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>23</v>
@@ -1098,7 +1098,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1112,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>41</v>
@@ -1127,7 +1127,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1141,7 +1141,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>42</v>
@@ -1156,7 +1156,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1170,7 +1170,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>43</v>
@@ -1185,7 +1185,7 @@
         <v>9</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1199,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>44</v>
@@ -1214,7 +1214,7 @@
         <v>9</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1228,7 +1228,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>45</v>
@@ -1243,7 +1243,7 @@
         <v>9</v>
       </c>
       <c r="I12" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1257,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>46</v>
@@ -1272,7 +1272,7 @@
         <v>9</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1287,13 +1287,13 @@
         <v>117</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>108</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>110</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>11</v>
@@ -1302,7 +1302,7 @@
         <v>9</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1316,13 +1316,13 @@
         <v>27</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>11</v>
@@ -1331,7 +1331,7 @@
         <v>9</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1339,19 +1339,19 @@
         <v>10</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C16" s="18">
         <v>1</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E16" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>85</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>87</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>11</v>
@@ -1360,7 +1360,7 @@
         <v>9</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1368,28 +1368,28 @@
         <v>11</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17" s="18">
         <v>3</v>
       </c>
       <c r="D17" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="H17" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1403,22 +1403,22 @@
         <v>1</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>103</v>
-      </c>
       <c r="H18" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1432,22 +1432,22 @@
         <v>1</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>107</v>
-      </c>
       <c r="H19" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1476,7 +1476,7 @@
         <v>9</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1505,7 +1505,7 @@
         <v>9</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1534,7 +1534,7 @@
         <v>9</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1563,7 +1563,7 @@
         <v>9</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1592,7 +1592,7 @@
         <v>9</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1606,51 +1606,51 @@
         <v>13</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>69</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H25" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="18">
         <v>20</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C26" s="18">
         <v>1</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>84</v>
+      <c r="E26" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1664,16 +1664,16 @@
         <v>1</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H27" s="20" t="s">
         <v>9</v>
@@ -1691,16 +1691,16 @@
         <v>1</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E28" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="H28" s="19" t="s">
         <v>9</v>
@@ -1718,22 +1718,22 @@
         <v>1</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H29" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I29" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1747,13 +1747,13 @@
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>16</v>
@@ -1780,16 +1780,16 @@
         <v>20</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H31" s="20" t="s">
         <v>9</v>
       </c>
       <c r="I31" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1803,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>50</v>
@@ -1818,7 +1818,7 @@
         <v>9</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1826,28 +1826,28 @@
         <v>27</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1861,22 +1861,22 @@
         <v>2</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1884,28 +1884,28 @@
         <v>29</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C35" s="17">
         <v>1</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1913,6 +1913,10 @@
     </row>
     <row r="37" spans="1:9">
       <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>